<commit_message>
Add Ingredients tables in Sample Recipes file
</commit_message>
<xml_diff>
--- a/Sample Recipes.xlsx
+++ b/Sample Recipes.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kianzhong\Documents\AY2324\VIA\mealprep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B29B88A-B9F1-4C5D-A1C5-EB7C8BD898CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6759E2DA-C0D0-4C9C-BA89-C0497425E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" xr2:uid="{A03220F9-C8D7-4DCD-A101-5AC7479E2ED3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Full Recipes" sheetId="1" r:id="rId1"/>
+    <sheet name="Ingredients for Recipe 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Ingredients for Recipe 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Issues and Insights" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
   <si>
     <t>Sample Recipes</t>
   </si>
@@ -96,12 +99,204 @@
   <si>
     <t>https://www.youtube.com/watch?v=AYXfaVD5o40</t>
   </si>
+  <si>
+    <t>No.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Quantity </t>
+  </si>
+  <si>
+    <t>Unit of measurement</t>
+  </si>
+  <si>
+    <t>Ingredient name in recipe</t>
+  </si>
+  <si>
+    <t>Number of units needed</t>
+  </si>
+  <si>
+    <t>Price per unit</t>
+  </si>
+  <si>
+    <t>Quantity per unit</t>
+  </si>
+  <si>
+    <t>Total price for ingredient</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Chicken breast</t>
+  </si>
+  <si>
+    <t>1b</t>
+  </si>
+  <si>
+    <t>1a</t>
+  </si>
+  <si>
+    <t>Pork tenderloin</t>
+  </si>
+  <si>
+    <t>Salt</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Pepper</t>
+  </si>
+  <si>
+    <t>Herbs or aromatics</t>
+  </si>
+  <si>
+    <t>Cooking spray</t>
+  </si>
+  <si>
+    <t>ml (1 tablespoon)</t>
+  </si>
+  <si>
+    <t>Photo of product</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Ground turkey</t>
+  </si>
+  <si>
+    <t>Sage</t>
+  </si>
+  <si>
+    <t>Onion Powder</t>
+  </si>
+  <si>
+    <t>Garlic powder</t>
+  </si>
+  <si>
+    <t>Fine sea salt</t>
+  </si>
+  <si>
+    <t>Cayenne powder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Black pepper </t>
+  </si>
+  <si>
+    <t>Slices</t>
+  </si>
+  <si>
+    <t>Whole wheat bread</t>
+  </si>
+  <si>
+    <t>Fresh eggs</t>
+  </si>
+  <si>
+    <t>Name of closest matching product</t>
+  </si>
+  <si>
+    <t>Supermarket doesn't have ingredients needed</t>
+  </si>
+  <si>
+    <t>Unit of measurement used in supermarket is different from recipes</t>
+  </si>
+  <si>
+    <t>Issue/Insights</t>
+  </si>
+  <si>
+    <t>*Promotion pricing of 6.95 for 2 packets</t>
+  </si>
+  <si>
+    <t>Ballgus Turkey Ham</t>
+  </si>
+  <si>
+    <t>Immediate solutions/Possible work-arounds</t>
+  </si>
+  <si>
+    <t>Ideal solution (future development)</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>Sourced from shengsiong.com.sg</t>
+  </si>
+  <si>
+    <t>Mccormick Garlic Powder</t>
+  </si>
+  <si>
+    <t>Add feature where users can track their inventory at home and be able to see how much ingredients they have left</t>
+  </si>
+  <si>
+    <t>Note promotional pricing, which will be cheaper than price calculated using unit price</t>
+  </si>
+  <si>
+    <t>Pagoda fine salt</t>
+  </si>
+  <si>
+    <t>Happy Family Black Pepper Powder</t>
+  </si>
+  <si>
+    <t>Estimated 14 slices of bread in 1 loaf</t>
+  </si>
+  <si>
+    <t>Sunshine Enriched Softmeal Whole Grain Bread</t>
+  </si>
+  <si>
+    <t>Total price:</t>
+  </si>
+  <si>
+    <t>Portion size may not fit user's needs</t>
+  </si>
+  <si>
+    <t>Add a feature which allow users to input their party size and scale the recipe quantities accordingly</t>
+  </si>
+  <si>
+    <t>Create a conversion table between different units of measurements, e.g. 1 egg ~= 60g</t>
+  </si>
+  <si>
+    <t>Calculate by unit price for the time being, in the proof-of-concept phase.</t>
+  </si>
+  <si>
+    <t>Avivar Frozen Chicken Breast</t>
+  </si>
+  <si>
+    <t>Australia Pork Fillet</t>
+  </si>
+  <si>
+    <t>Ingredients may have different names in different countries and cultures</t>
+  </si>
+  <si>
+    <t>Create a table of synonyms for commonly used ingredients</t>
+  </si>
+  <si>
+    <t>Knife Cooking Oil</t>
+  </si>
+  <si>
+    <t>The same ingredients (Same brand as well) may have different sizes</t>
+  </si>
+  <si>
+    <t>The same ingredients may have more than 1 brand carry it</t>
+  </si>
+  <si>
+    <t>MasterFoods Mixed Herbs</t>
+  </si>
+  <si>
+    <t>Used cooking oil to substitue</t>
+  </si>
+  <si>
+    <t>Find the next best product that best matches the original ingredient</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +308,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -154,7 +357,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -175,6 +378,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -191,6 +416,744 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241301</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1325034</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1134533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Avivar Frozen Chicken Breast">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D871D08-B62D-96D5-B210-4F9C98C909FE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4466168" y="960967"/>
+          <a:ext cx="1083733" cy="1083733"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>194735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1329266</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>902511</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr=" Australia Pork Fillet">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A415DA8-AB8F-9AC1-A3F3-4FAFF53FE8EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="13623" t="26376" r="13140" b="30049"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4275667" y="2247902"/>
+          <a:ext cx="1189566" cy="707776"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>220134</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>80434</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1413933</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>1274233</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Pagoda Fine Salt">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B38B4F90-AEFB-4EE3-8DDD-0F2877438AAF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4356101" y="3276601"/>
+          <a:ext cx="1193799" cy="1193799"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>279401</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1231899</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>986365</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4" descr="Happy Family Black Pepper Powder">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{65CFEB8F-FD20-4C9B-ADE3-A69C4D265DB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4415368" y="4601634"/>
+          <a:ext cx="952498" cy="952498"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>118534</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1172633</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1049867</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Knife Cooking Oil">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{650086E9-2B00-DEC2-0BF3-4C797DFD250F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4377267" y="6972301"/>
+          <a:ext cx="931333" cy="931333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>296332</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>135466</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1227665</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1066799</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="MasterFoods Mixed Herbs">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5D097273-14A3-9B9E-913C-783B4AA75DBD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4432299" y="5846233"/>
+          <a:ext cx="931333" cy="931333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>207434</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>402166</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1426634</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>1155700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2" descr=" Fresh Eggs">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D3671165-5942-4712-B993-CFDCE7BF1FBF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect t="25320" b="29156"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3771901" y="948266"/>
+          <a:ext cx="1219200" cy="753534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>283634</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>46568</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1397000</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>1159934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3" descr="Ballgus Turkey Ham">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D842C36E-4F00-3DBB-1C3F-01F3E316BBA7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3848101" y="2175935"/>
+          <a:ext cx="1113366" cy="1113366"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>347134</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>249767</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1358900</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>1261533</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5" descr="Mccormick Garlic Powder">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8AE2A3A7-21D6-6A07-33D5-B42C3916CC64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4135967" y="4220634"/>
+          <a:ext cx="1011766" cy="1011766"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>215901</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1528235</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>1439334</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6" descr="Pagoda Fine Salt">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C6F1D2C-C2A5-4A2A-8A70-69CBB1B18AFE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4097868" y="5808133"/>
+          <a:ext cx="1312334" cy="1312334"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>160868</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>80434</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1494368</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>1413934</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7" descr="Happy Family Black Pepper Powder">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{749CB292-04D0-8CA3-0426-7B2992DC6745}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4042835" y="8818034"/>
+          <a:ext cx="1333500" cy="1333500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>156635</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>67733</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1485901</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>1397000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8" descr="Sunshine Enriched Softmeal Whole Grain Bread">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3F254B42-34F1-E3E3-FF90-FA618144DEB7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4038602" y="10333566"/>
+          <a:ext cx="1329266" cy="1329267"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -492,8 +1455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B4753-CBB9-4FC6-84B7-FFE3841E6409}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -569,4 +1532,761 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFB0278D-C709-42C5-B1B9-8ADA32AD96F0}">
+  <dimension ref="A1:L11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="8.9375" style="9"/>
+    <col min="2" max="2" width="13.76171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.9375" style="9"/>
+    <col min="4" max="4" width="11.703125" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1171875" style="9" customWidth="1"/>
+    <col min="6" max="6" width="21.05859375" style="9" customWidth="1"/>
+    <col min="7" max="7" width="14.29296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.703125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="12.05859375" style="9" customWidth="1"/>
+    <col min="10" max="10" width="20.46875" style="9" customWidth="1"/>
+    <col min="11" max="16384" width="8.9375" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="A1" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="15" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4"/>
+      <c r="G4" s="9">
+        <v>2</v>
+      </c>
+      <c r="H4" s="9">
+        <f>ROUNDUP(C4/G4,0)</f>
+        <v>2</v>
+      </c>
+      <c r="I4" s="9">
+        <v>11.95</v>
+      </c>
+      <c r="J4" s="9">
+        <f>I4*H4</f>
+        <v>23.9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="9">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5"/>
+      <c r="G5" s="9">
+        <v>0.25</v>
+      </c>
+      <c r="H5" s="9">
+        <f t="shared" ref="H5:H9" si="0">ROUNDUP(C5/G5,0)</f>
+        <v>9</v>
+      </c>
+      <c r="I5" s="9">
+        <v>7.95</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:J9" si="1">I5*H5</f>
+        <v>71.55</v>
+      </c>
+      <c r="K5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="14">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="9">
+        <v>2</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6"/>
+      <c r="G6">
+        <v>500</v>
+      </c>
+      <c r="H6" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="J6" s="9">
+        <f t="shared" si="1"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A7" s="14">
+        <v>3</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="9">
+        <v>2</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F7"/>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I7" s="9">
+        <v>1.96</v>
+      </c>
+      <c r="J7" s="9">
+        <f t="shared" si="1"/>
+        <v>1.96</v>
+      </c>
+      <c r="L7" s="11"/>
+    </row>
+    <row r="8" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="14">
+        <v>4</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8"/>
+      <c r="G8" s="9">
+        <v>10</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>3.93</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="1"/>
+        <v>3.93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="14">
+        <v>5</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="9">
+        <v>15</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9"/>
+      <c r="G9" s="9">
+        <v>1000</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>4.79</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="1"/>
+        <v>4.79</v>
+      </c>
+      <c r="K9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="L9" s="11"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="I10" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="9">
+        <f>SUM(J4:J9)</f>
+        <v>106.83</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.5">
+      <c r="L11" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D522693-A951-45B8-91D1-7B315588885D}">
+  <dimension ref="A1:K13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="8.9375" style="9"/>
+    <col min="2" max="2" width="13.76171875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.9375" style="9"/>
+    <col min="4" max="4" width="12.05859375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="13.41015625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="24.41015625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="14.29296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.8203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.29296875" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.46875" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.05859375" style="9" customWidth="1"/>
+    <col min="12" max="16384" width="8.9375" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A1" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="15" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="115.35" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A4" s="14">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="9">
+        <v>7</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="G4" s="9">
+        <v>10</v>
+      </c>
+      <c r="H4" s="9">
+        <f>ROUNDUP(C4/G4,0)</f>
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>2.75</v>
+      </c>
+      <c r="J4" s="9">
+        <f>H4*I4</f>
+        <v>2.75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="97" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A5" s="14">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="9">
+        <v>900</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="G5" s="9">
+        <v>200</v>
+      </c>
+      <c r="H5" s="9">
+        <f>ROUNDUP(C5/G5,0)</f>
+        <v>5</v>
+      </c>
+      <c r="I5" s="9">
+        <v>3.83</v>
+      </c>
+      <c r="J5" s="9">
+        <f t="shared" ref="J5:J12" si="0">H5*I5</f>
+        <v>19.149999999999999</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A6" s="14">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="9">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="9" t="e">
+        <f t="shared" ref="H6:H12" si="1">ROUNDUP(C6/G6,0)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K6" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A7" s="14">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="9">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="9" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A8" s="14">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C8" s="9">
+        <v>8</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="9">
+        <v>88</v>
+      </c>
+      <c r="H8" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I8" s="9">
+        <v>9.48</v>
+      </c>
+      <c r="J8" s="9">
+        <f t="shared" si="0"/>
+        <v>9.48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="14">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" s="9">
+        <v>12</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="9">
+        <v>500</v>
+      </c>
+      <c r="H9" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I9" s="9">
+        <v>0.7</v>
+      </c>
+      <c r="J9" s="9">
+        <f t="shared" si="0"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A10" s="14">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" s="9" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A11" s="14">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="G11" s="9">
+        <v>35</v>
+      </c>
+      <c r="H11" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I11" s="9">
+        <v>1.96</v>
+      </c>
+      <c r="J11" s="9">
+        <f t="shared" si="0"/>
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A12" s="14">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C12" s="9">
+        <v>14</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G12" s="9">
+        <v>14</v>
+      </c>
+      <c r="H12" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I12" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="J12" s="9">
+        <f t="shared" si="0"/>
+        <v>3.1</v>
+      </c>
+      <c r="K12" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="I13" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="J13" s="9">
+        <f>SUM(J4:J12)</f>
+        <v>37.14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B385A7-E930-474B-A652-086B5E863EAA}">
+  <dimension ref="A3:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="1" max="1" width="8.9375" style="8"/>
+    <col min="2" max="2" width="61.05859375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.41015625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="30" style="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A4" s="8">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+      <c r="A5" s="8">
+        <v>2</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A7" s="8">
+        <v>4</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="43" x14ac:dyDescent="0.5">
+      <c r="A8" s="8">
+        <v>5</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A9" s="8">
+        <v>6</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A10" s="8">
+        <v>7</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A11" s="8">
+        <v>8</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Issues and Solutions table in Sample Recipes file
</commit_message>
<xml_diff>
--- a/Sample Recipes.xlsx
+++ b/Sample Recipes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kianzhong\Documents\AY2324\VIA\mealprep\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6759E2DA-C0D0-4C9C-BA89-C0497425E56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C961EFDE-94C7-4511-A9D2-4EF0A6BFE1E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" xr2:uid="{A03220F9-C8D7-4DCD-A101-5AC7479E2ED3}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20186" windowHeight="12800" activeTab="3" xr2:uid="{A03220F9-C8D7-4DCD-A101-5AC7479E2ED3}"/>
   </bookViews>
   <sheets>
     <sheet name="Full Recipes" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="84">
   <si>
     <t>Sample Recipes</t>
   </si>
@@ -253,9 +253,6 @@
     <t>Portion size may not fit user's needs</t>
   </si>
   <si>
-    <t>Add a feature which allow users to input their party size and scale the recipe quantities accordingly</t>
-  </si>
-  <si>
     <t>Create a conversion table between different units of measurements, e.g. 1 egg ~= 60g</t>
   </si>
   <si>
@@ -289,7 +286,30 @@
     <t>Used cooking oil to substitue</t>
   </si>
   <si>
-    <t>Find the next best product that best matches the original ingredient</t>
+    <t>Calculate the unit prices and present it to user?</t>
+  </si>
+  <si>
+    <t>Perhaps we can develop a in-app shopping function</t>
+  </si>
+  <si>
+    <t>Find the next best product that best matches the original ingredient, if not, specify not available</t>
+  </si>
+  <si>
+    <t>Give options to choose between metric and us based measurements</t>
+  </si>
+  <si>
+    <t>Have to included serving size for recipes</t>
+  </si>
+  <si>
+    <t>Add a feature which allow users to input their party size and scale the recipe quantities accordingly
+When recipe owners input their recipes, include fields where they can enter</t>
+  </si>
+  <si>
+    <t>Have to brainstorm a few options</t>
+  </si>
+  <si>
+    <t>List out all options for the ingredients available within selected supermarket
+Perhaps we can shortlist 3</t>
   </si>
 </sst>
 </file>
@@ -357,7 +377,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -372,19 +392,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -398,6 +411,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1455,7 +1474,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D8B4753-CBB9-4FC6-84B7-FFE3841E6409}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B4" sqref="B4:B5"/>
     </sheetView>
   </sheetViews>
@@ -1490,7 +1509,7 @@
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="13" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1504,7 +1523,7 @@
       <c r="A5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
@@ -1544,265 +1563,265 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.9375" style="9"/>
-    <col min="2" max="2" width="13.76171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.9375" style="9"/>
-    <col min="4" max="4" width="11.703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1171875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="21.05859375" style="9" customWidth="1"/>
-    <col min="7" max="7" width="14.29296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.703125" style="9" customWidth="1"/>
-    <col min="9" max="9" width="12.05859375" style="9" customWidth="1"/>
-    <col min="10" max="10" width="20.46875" style="9" customWidth="1"/>
-    <col min="11" max="16384" width="8.9375" style="9"/>
+    <col min="1" max="1" width="8.9375" style="7"/>
+    <col min="2" max="2" width="13.76171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.9375" style="7"/>
+    <col min="4" max="4" width="11.703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1171875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="21.05859375" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.29296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.703125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="12.05859375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="20.46875" style="7" customWidth="1"/>
+    <col min="11" max="16384" width="8.9375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:12" s="15" customFormat="1" ht="43" x14ac:dyDescent="0.5">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:12" s="12" customFormat="1" ht="43" x14ac:dyDescent="0.5">
+      <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>68</v>
+      <c r="E4" s="7" t="s">
+        <v>67</v>
       </c>
       <c r="F4"/>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>2</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <f>ROUNDUP(C4/G4,0)</f>
         <v>2</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>11.95</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <f>I4*H4</f>
         <v>23.9</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>69</v>
+      <c r="E5" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="F5"/>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>0.25</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <f t="shared" ref="H5:H9" si="0">ROUNDUP(C5/G5,0)</f>
         <v>9</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>7.95</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <f t="shared" ref="J5:J9" si="1">I5*H5</f>
         <v>71.55</v>
       </c>
       <c r="K5" s="3"/>
     </row>
     <row r="6" spans="1:12" ht="108" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="14">
+      <c r="A6" s="11">
         <v>2</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>2</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>59</v>
       </c>
       <c r="F6"/>
       <c r="G6">
         <v>500</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>0.7</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <f t="shared" si="1"/>
         <v>0.7</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="14">
+      <c r="A7" s="11">
         <v>3</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>2</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>60</v>
       </c>
       <c r="F7"/>
       <c r="G7">
         <v>35</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I7" s="9">
+      <c r="I7" s="7">
         <v>1.96</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="7">
         <f t="shared" si="1"/>
         <v>1.96</v>
       </c>
-      <c r="L7" s="11"/>
+      <c r="L7" s="8"/>
     </row>
     <row r="8" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="14">
+      <c r="A8" s="11">
         <v>4</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>0.5</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="9" t="s">
-        <v>75</v>
+      <c r="E8" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="F8"/>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>10</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>3.93</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f t="shared" si="1"/>
         <v>3.93</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="90" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="14">
+      <c r="A9" s="11">
         <v>5</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>15</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="9" t="s">
-        <v>72</v>
+      <c r="E9" s="7" t="s">
+        <v>71</v>
       </c>
       <c r="F9"/>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>1000</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>4.79</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="7">
         <f t="shared" si="1"/>
         <v>4.79</v>
       </c>
-      <c r="K9" s="9" t="s">
-        <v>76</v>
-      </c>
-      <c r="L9" s="11"/>
+      <c r="K9" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="7">
         <f>SUM(J4:J9)</f>
         <v>106.83</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.5">
-      <c r="L11" s="11"/>
+      <c r="L11" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1815,120 +1834,120 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.9375" style="9"/>
-    <col min="2" max="2" width="13.76171875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.9375" style="9"/>
-    <col min="4" max="4" width="12.05859375" style="9" customWidth="1"/>
-    <col min="5" max="5" width="13.41015625" style="9" customWidth="1"/>
-    <col min="6" max="6" width="24.41015625" style="9" customWidth="1"/>
-    <col min="7" max="7" width="14.29296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.8203125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.29296875" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.46875" style="9" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.05859375" style="9" customWidth="1"/>
-    <col min="12" max="16384" width="8.9375" style="9"/>
+    <col min="1" max="1" width="8.9375" style="7"/>
+    <col min="2" max="2" width="13.76171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.9375" style="7"/>
+    <col min="4" max="4" width="12.05859375" style="7" customWidth="1"/>
+    <col min="5" max="5" width="13.41015625" style="7" customWidth="1"/>
+    <col min="6" max="6" width="24.41015625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="14.29296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.8203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.29296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.46875" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.05859375" style="7" customWidth="1"/>
+    <col min="12" max="16384" width="8.9375" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A1" s="10" t="s">
+      <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="15" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
-      <c r="A3" s="15" t="s">
+    <row r="3" spans="1:11" s="12" customFormat="1" ht="57.35" x14ac:dyDescent="0.5">
+      <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="15" t="s">
+      <c r="H3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="15" t="s">
+      <c r="J3" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="115.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="14">
+      <c r="A4" s="11">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="7">
         <v>7</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>10</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <f>ROUNDUP(C4/G4,0)</f>
         <v>1</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>2.75</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <f>H4*I4</f>
         <v>2.75</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="97" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A5" s="14">
+      <c r="A5" s="11">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="7">
         <v>900</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="7">
         <v>200</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="7">
         <f>ROUNDUP(C5/G5,0)</f>
         <v>5</v>
       </c>
-      <c r="I5" s="9">
+      <c r="I5" s="7">
         <v>3.83</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="7">
         <f t="shared" ref="J5:J12" si="0">H5*I5</f>
         <v>19.149999999999999</v>
       </c>
@@ -1937,236 +1956,236 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A6" s="14">
+      <c r="A6" s="11">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="9" t="e">
+      <c r="H6" s="7" t="e">
         <f t="shared" ref="H6:H12" si="1">ROUNDUP(C6/G6,0)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="A7" s="14">
+      <c r="A7" s="11">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="7">
         <v>1</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="9" t="e">
+      <c r="H7" s="7" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="I7" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="9" t="s">
+      <c r="K7" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="14">
+      <c r="A8" s="11">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="7">
         <v>8</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="7">
         <v>88</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I8" s="9">
+      <c r="I8" s="7">
         <v>9.48</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="7">
         <f t="shared" si="0"/>
         <v>9.48</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="14">
+      <c r="A9" s="11">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="7">
         <v>12</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="7">
         <v>500</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I9" s="9">
+      <c r="I9" s="7">
         <v>0.7</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="7">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A10" s="14">
+      <c r="A10" s="11">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="7">
         <v>0.5</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="9" t="e">
+      <c r="H10" s="7" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="I10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K10" s="9" t="s">
+      <c r="K10" s="7" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="14">
+      <c r="A11" s="11">
         <v>8</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="7">
         <v>0.5</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="7">
         <v>35</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I11" s="9">
+      <c r="I11" s="7">
         <v>1.96</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="7">
         <f t="shared" si="0"/>
         <v>1.96</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="120.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A12" s="14">
+      <c r="A12" s="11">
         <v>9</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="7">
         <v>14</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="7">
         <v>14</v>
       </c>
-      <c r="H12" s="9">
+      <c r="H12" s="7">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I12" s="9">
+      <c r="I12" s="7">
         <v>3.1</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="7">
         <f t="shared" si="0"/>
         <v>3.1</v>
       </c>
-      <c r="K12" s="9" t="s">
+      <c r="K12" s="7" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.5">
-      <c r="I13" s="9" t="s">
+      <c r="I13" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="7">
         <f>SUM(J4:J12)</f>
         <v>37.14</v>
       </c>
@@ -2179,111 +2198,129 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56B385A7-E930-474B-A652-086B5E863EAA}">
-  <dimension ref="A3:D11"/>
+  <dimension ref="A3:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="8.9375" style="8"/>
-    <col min="2" max="2" width="61.05859375" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.41015625" style="9" customWidth="1"/>
-    <col min="4" max="4" width="30" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.9375" style="6"/>
+    <col min="2" max="2" width="61.05859375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.41015625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="30" style="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
+      <c r="A3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A4" s="8">
+    <row r="4" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A4" s="6">
         <v>1</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="7" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="43" x14ac:dyDescent="0.5">
-      <c r="A5" s="8">
+    <row r="5" spans="1:5" ht="43" x14ac:dyDescent="0.5">
+      <c r="A5" s="6">
         <v>2</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="C5" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A6" s="8">
-        <v>3</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A7" s="8">
+    <row r="7" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A7" s="6">
         <v>4</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="7" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="43" x14ac:dyDescent="0.5">
-      <c r="A8" s="8">
+    <row r="8" spans="1:5" ht="100.35" x14ac:dyDescent="0.5">
+      <c r="A8" s="6">
         <v>5</v>
       </c>
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.7" x14ac:dyDescent="0.5">
-      <c r="A9" s="8">
+      <c r="C8" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A9" s="6">
         <v>6</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A10" s="8">
+    </row>
+    <row r="10" spans="1:5" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="43" x14ac:dyDescent="0.5">
+      <c r="A11" s="6">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.5">
-      <c r="A11" s="8">
-        <v>8</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>74</v>
+      <c r="C11" s="7" t="s">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>